<commit_message>
Everything should reflect Ziptie Design 4 for the Toaster Charger PCB. Appropriate CAD files have been provided. Pictures of a rough draft, done with components carefully placed on a to-scale printout of the board included. Gerber files generated for both basic and advanced prototype purposes.
</commit_message>
<xml_diff>
--- a/hardware/ELEC/ToasterChargerModule/DigikeyPartsOrder.xlsx
+++ b/hardware/ELEC/ToasterChargerModule/DigikeyPartsOrder.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>All prices are in US dollars.</t>
   </si>
@@ -163,6 +163,81 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>490-7207-1-ND </t>
+  </si>
+  <si>
+    <t>GRM219R61E106KA12D</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V 10% X5R 0805</t>
+  </si>
+  <si>
+    <t>193,908 - Immediate</t>
+  </si>
+  <si>
+    <t>Cut Tape (CT)  </t>
+  </si>
+  <si>
+    <t>Alternate Packaging</t>
+  </si>
+  <si>
+    <t>GRM</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>±10%</t>
+  </si>
+  <si>
+    <t>25V</t>
+  </si>
+  <si>
+    <t>X5R</t>
+  </si>
+  <si>
+    <t>Surface Mount, MLCC</t>
+  </si>
+  <si>
+    <t>-55°C ~ 85°C</t>
+  </si>
+  <si>
+    <t>General Purpose</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>0.079" L x 0.049" W (2.01mm x 1.25mm)</t>
+  </si>
+  <si>
+    <t>0.037" (0.95mm)</t>
+  </si>
+  <si>
+    <t>Good to test</t>
+  </si>
+  <si>
+    <t>Good to test, but have to change PCB footprint.</t>
+  </si>
+  <si>
+    <t>Good to test (I think)</t>
+  </si>
+  <si>
+    <t>Seems okay</t>
+  </si>
+  <si>
+    <t>Seems fine</t>
+  </si>
+  <si>
+    <t>Replace 10 with</t>
   </si>
 </sst>
 </file>
@@ -172,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +282,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -228,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -498,12 +579,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -559,6 +677,99 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -568,98 +779,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1753,7 +1925,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1780,6 +1952,234 @@
         <a:xfrm>
           <a:off x="1219200" y="4008120"/>
           <a:ext cx="609600" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="GRM219R61E106KA12D Datasheet">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21" tgtFrame="_blank"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7315200" y="4191000"/>
+          <a:ext cx="342900" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22" descr="GRM219R61E106KA12D - Murata Electronics North America">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7924800" y="4191000"/>
+          <a:ext cx="609600" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23" descr="This part is RoHS compliant.">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8534400" y="4191000"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24" descr="?">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12801600" y="4191000"/>
+          <a:ext cx="152400" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2089,29 +2489,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
     </row>
-    <row r="2" spans="1:10" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2143,461 +2543,622 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="26" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="29">
         <v>0</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="31">
         <v>0.94</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="33">
         <v>0.94</v>
       </c>
+      <c r="K3" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="42"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="31"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="36" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="37">
         <v>0</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="19">
         <v>9.2799999999999994</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="21">
         <v>18.559999999999999</v>
       </c>
+      <c r="K5" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="36"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="41"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="22"/>
     </row>
-    <row r="7" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="29">
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="31">
         <v>1.21</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="33">
         <v>2.42</v>
       </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="42"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="31"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="36" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="4">
         <v>10</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="37">
         <v>0</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="19">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="21">
         <v>0.11</v>
       </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="36"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
       <c r="G10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="41"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="22"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="26" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="29">
         <v>0</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="31">
         <v>0.63</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="33">
         <v>3.15</v>
       </c>
+      <c r="K11" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="42"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="31"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="36" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="4">
         <v>5</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="37">
         <v>0</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="19">
         <v>0.1</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="21">
         <v>0.5</v>
       </c>
+      <c r="K13" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="36"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="35"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="41"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="22"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="26" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="2">
         <v>2</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="29">
         <v>0</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="31">
         <v>3.65</v>
       </c>
-      <c r="J15" s="30">
+      <c r="J15" s="33">
         <v>7.3</v>
       </c>
+      <c r="K15" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="46"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
       <c r="G16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="46"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="45"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
+    <row r="17" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="42"/>
       <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="31"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="34"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="32" t="s">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="36" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="4">
         <v>5</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="37">
         <v>0</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="19">
         <v>0.1</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="21">
         <v>0.5</v>
       </c>
+      <c r="K18" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
+    <row r="19" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="36"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="35"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="41"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="22"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="2">
         <v>2</v>
       </c>
-      <c r="H20" s="24">
+      <c r="H20" s="29">
         <v>0</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="31">
         <v>0.77</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="33">
         <v>1.54</v>
       </c>
+      <c r="K20" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+    <row r="21" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="42"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="31"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="34"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="32" t="s">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="36" t="s">
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="34"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="4">
         <v>2</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="37">
         <v>0</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="19">
         <v>0.17</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="21">
         <v>0.34</v>
       </c>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="33"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
+    <row r="23" spans="1:38" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="36"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
       <c r="G23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="41"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="22"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="P23" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q23" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="R23" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="S23" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="T23" s="68">
+        <v>0.26</v>
+      </c>
+      <c r="U23" s="56">
+        <v>2</v>
+      </c>
+      <c r="V23" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="W23" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="X23" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y23" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z23" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA23" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB23" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC23" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD23" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE23" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF23" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG23" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH23" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI23" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ23" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK23" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL23" s="56" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
+    <row r="24" spans="1:38" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
       <c r="I24" s="10" t="s">
         <v>43</v>
       </c>
       <c r="J24" s="14">
         <v>35.36</v>
       </c>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="W24" s="69"/>
+      <c r="X24" s="57"/>
+      <c r="Y24" s="57"/>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="57"/>
+      <c r="AB24" s="57"/>
+      <c r="AC24" s="57"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="57"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="57"/>
+      <c r="AI24" s="57"/>
+      <c r="AJ24" s="57"/>
+      <c r="AK24" s="57"/>
+      <c r="AL24" s="57"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
       <c r="I25" s="10" t="s">
         <v>44</v>
       </c>
       <c r="J25" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="70"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="70"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="58"/>
+      <c r="AC25" s="58"/>
+      <c r="AD25" s="58"/>
+      <c r="AE25" s="58"/>
+      <c r="AF25" s="58"/>
+      <c r="AG25" s="58"/>
+      <c r="AH25" s="58"/>
+      <c r="AI25" s="58"/>
+      <c r="AJ25" s="58"/>
+      <c r="AK25" s="58"/>
+      <c r="AL25" s="58"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="11" t="s">
         <v>46</v>
       </c>
@@ -2605,15 +3166,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
+    <row r="27" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="17" t="s">
         <v>48</v>
       </c>
@@ -2621,19 +3182,113 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="94">
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
+  <mergeCells count="120">
+    <mergeCell ref="AL23:AL25"/>
+    <mergeCell ref="AG23:AG25"/>
+    <mergeCell ref="AH23:AH25"/>
+    <mergeCell ref="AI23:AI25"/>
+    <mergeCell ref="AJ23:AJ25"/>
+    <mergeCell ref="AK23:AK25"/>
+    <mergeCell ref="AB23:AB25"/>
+    <mergeCell ref="AC23:AC25"/>
+    <mergeCell ref="AD23:AD25"/>
+    <mergeCell ref="AE23:AE25"/>
+    <mergeCell ref="AF23:AF25"/>
+    <mergeCell ref="W23:W25"/>
+    <mergeCell ref="X23:X25"/>
+    <mergeCell ref="Y23:Y25"/>
+    <mergeCell ref="Z23:Z25"/>
+    <mergeCell ref="AA23:AA25"/>
+    <mergeCell ref="Q23:Q25"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="S23:S25"/>
+    <mergeCell ref="T23:T25"/>
+    <mergeCell ref="U23:U25"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="P23:P25"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="H20:H21"/>
     <mergeCell ref="I20:I21"/>
@@ -2650,79 +3305,11 @@
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="javascript:__doPostBack('ctl00$ctl00$mainContentPlaceHolder$mainContentPlaceHolder$ordOrderDetails$detailRow_161096401$lnkDelete_161096401','')"/>
@@ -2748,10 +3335,16 @@
     <hyperlink ref="D22" r:id="rId21" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=161115790&amp;uq=635514902842382440&amp;CSRT=1372573990585885048"/>
     <hyperlink ref="J25" r:id="rId22" display="http://www.digikey.com/classic/Ordering/ShipCostEstimator.aspx?ReturnURL=/classic/ordering/addpart.aspx&amp;PopUp=true&amp;CSRT=1372573990585885048"/>
     <hyperlink ref="I26" r:id="rId23" display="http://www.digikey.com/classic/Help.aspx?id=Sales%20Tax%20Help&amp;CSRT=1372573990585885048"/>
+    <hyperlink ref="P23" r:id="rId24" display="http://www.digikey.com/product-detail/en/GRM219R61E106KA12D/490-7207-1-ND/3900481"/>
+    <hyperlink ref="Q23" r:id="rId25" display="http://digikey.com/Suppliers/us/Murata-Electronics.page?lang=en"/>
+    <hyperlink ref="T23" r:id="rId26" display="http://www.digikey.com/product-detail/en/GRM219R61E106KA12D/490-7207-1-ND/3900481"/>
+    <hyperlink ref="V23" r:id="rId27" display="javascript:dlgHelp('Cut Tape Help');"/>
+    <hyperlink ref="V24" r:id="rId28" display="http://www.digikey.com/scripts/dksearch/dksus.dll?AlternatePackaging&amp;name=490-7207-1-ND"/>
+    <hyperlink ref="W23" r:id="rId29" display="http://www.digikey.com/product-search/en?FV=ffec150e"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId24"/>
-  <drawing r:id="rId25"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId30"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>